<commit_message>
fetch data through the files(stations)
</commit_message>
<xml_diff>
--- a/Home/ARG.xlsx
+++ b/Home/ARG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="OPERATINAL" sheetId="1" r:id="rId1"/>
@@ -926,13 +926,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2153,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>